<commit_message>
Kunde läsa in energi i excel men inte scatter power
</commit_message>
<xml_diff>
--- a/MC_Linnea/Monte Carlo, test.xlsx
+++ b/MC_Linnea/Monte Carlo, test.xlsx
@@ -3,16 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28417"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="345" documentId="11_3D4F55BF84DCCE036F15A6DB9431F45B9AFF0E61" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E3D923E9-E29F-4837-8DE4-4C1C650BDD21}"/>
+  <xr:revisionPtr revIDLastSave="346" documentId="11_3D4F55BF84DCCE036F15A6DB9431F45B9AFF0E61" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B600BE0B-0876-4E80-AFF9-D6DB2D203E15}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kladd" sheetId="1" r:id="rId1"/>
     <sheet name="Scattering power" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Scattering power'!$A$3:$B$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Scattering power'!$A$1:$B$18</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -4321,8 +4321,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:AK35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AI1" sqref="AI1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4968,10 +4968,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF36332B-B747-420B-84FA-C4CB3A896F1E}">
-  <dimension ref="A3:F36"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4987,15 +4987,39 @@
     <col min="10" max="10" width="23.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="B2" s="9">
+        <v>5910</v>
+      </c>
+      <c r="C2" s="8">
+        <f>A2*10^6</f>
+        <v>10000</v>
+      </c>
+    </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>3</v>
+      <c r="A3" s="9">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="B3" s="9">
+        <v>2920</v>
+      </c>
+      <c r="C3" s="8">
+        <f>A3*10^6</f>
+        <v>15000</v>
       </c>
       <c r="F3" t="s">
         <v>18</v>
@@ -5003,402 +5027,378 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="9">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="B4" s="9">
-        <v>5910</v>
+        <v>1770</v>
       </c>
       <c r="C4" s="8">
         <f>A4*10^6</f>
-        <v>10000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="9">
-        <v>1.4999999999999999E-2</v>
+        <v>0.03</v>
       </c>
       <c r="B5" s="9">
-        <v>2920</v>
+        <v>869</v>
       </c>
       <c r="C5" s="8">
         <f>A5*10^6</f>
-        <v>15000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="9">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="B6" s="9">
-        <v>1770</v>
+        <v>516</v>
       </c>
       <c r="C6" s="8">
         <f>A6*10^6</f>
-        <v>20000</v>
+        <v>40000</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="9">
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
       <c r="B7" s="9">
-        <v>869</v>
+        <v>357</v>
       </c>
       <c r="C7" s="8">
         <f>A7*10^6</f>
-        <v>30000</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="9">
-        <v>0.04</v>
+        <v>0.06</v>
       </c>
       <c r="B8" s="9">
-        <v>516</v>
+        <v>261</v>
       </c>
       <c r="C8" s="8">
         <f>A8*10^6</f>
-        <v>40000</v>
+        <v>60000</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="9">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
       <c r="B9" s="9">
-        <v>357</v>
+        <v>159</v>
       </c>
       <c r="C9" s="8">
         <f>A9*10^6</f>
-        <v>50000</v>
+        <v>80000</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="9">
-        <v>0.06</v>
+        <v>0.1</v>
       </c>
       <c r="B10" s="9">
-        <v>261</v>
+        <v>109</v>
       </c>
       <c r="C10" s="8">
         <f>A10*10^6</f>
-        <v>60000</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="9">
-        <v>0.08</v>
+        <v>0.15</v>
       </c>
       <c r="B11" s="9">
-        <v>159</v>
+        <v>55.7</v>
       </c>
       <c r="C11" s="8">
         <f>A11*10^6</f>
-        <v>80000</v>
+        <v>150000</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="9">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="B12" s="9">
-        <v>109</v>
+        <v>35</v>
       </c>
       <c r="C12" s="8">
         <f>A12*10^6</f>
-        <v>100000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="9">
-        <v>0.15</v>
+        <v>0.3</v>
       </c>
       <c r="B13" s="9">
-        <v>55.7</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="C13" s="8">
         <f>A13*10^6</f>
-        <v>150000</v>
+        <v>300000</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="9">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="B14" s="9">
-        <v>35</v>
+        <v>11.8</v>
       </c>
       <c r="C14" s="8">
         <f>A14*10^6</f>
-        <v>200000</v>
+        <v>400000</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="9">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="B15" s="9">
-        <v>18.399999999999999</v>
+        <v>8.4499999999999993</v>
       </c>
       <c r="C15" s="8">
         <f>A15*10^6</f>
-        <v>300000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="9">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="B16" s="9">
-        <v>11.8</v>
+        <v>6.42</v>
       </c>
       <c r="C16" s="8">
         <f>A16*10^6</f>
-        <v>400000</v>
+        <v>600000</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="9">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="B17" s="9">
-        <v>8.4499999999999993</v>
+        <v>4.17</v>
       </c>
       <c r="C17" s="8">
         <f>A17*10^6</f>
-        <v>500000</v>
+        <v>800000</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="9">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="B18" s="9">
-        <v>6.42</v>
+        <v>2.99</v>
       </c>
       <c r="C18" s="8">
         <f>A18*10^6</f>
-        <v>600000</v>
+        <v>1000000</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="9">
-        <v>0.8</v>
+        <v>1.5</v>
       </c>
       <c r="B19" s="9">
-        <v>4.17</v>
+        <v>1.61</v>
       </c>
       <c r="C19" s="8">
         <f>A19*10^6</f>
-        <v>800000</v>
+        <v>1500000</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B20" s="9">
-        <v>2.99</v>
+        <v>1.03</v>
       </c>
       <c r="C20" s="8">
         <f>A20*10^6</f>
-        <v>1000000</v>
+        <v>2000000</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="9">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="B21" s="9">
-        <v>1.61</v>
+        <v>0.54</v>
       </c>
       <c r="C21" s="8">
         <f>A21*10^6</f>
-        <v>1500000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B22" s="9">
-        <v>1.03</v>
+        <v>0.33600000000000002</v>
       </c>
       <c r="C22" s="8">
         <f>A22*10^6</f>
-        <v>2000000</v>
+        <v>4000000</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="9">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B23" s="9">
-        <v>0.54</v>
+        <v>0.23100000000000001</v>
       </c>
       <c r="C23" s="8">
         <f>A23*10^6</f>
-        <v>3000000</v>
+        <v>5000000</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="9">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B24" s="9">
-        <v>0.33600000000000002</v>
+        <v>0.16900000000000001</v>
       </c>
       <c r="C24" s="8">
         <f>A24*10^6</f>
-        <v>4000000</v>
+        <v>6000000</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="9">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B25" s="9">
-        <v>0.23100000000000001</v>
+        <v>0.10299999999999999</v>
       </c>
       <c r="C25" s="8">
         <f>A25*10^6</f>
-        <v>5000000</v>
+        <v>8000000</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="9">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B26" s="9">
-        <v>0.16900000000000001</v>
+        <v>6.9500000000000006E-2</v>
       </c>
       <c r="C26" s="8">
         <f>A26*10^6</f>
-        <v>6000000</v>
+        <v>10000000</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="9">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B27" s="9">
-        <v>0.10299999999999999</v>
+        <v>3.3700000000000001E-2</v>
       </c>
       <c r="C27" s="8">
         <f>A27*10^6</f>
-        <v>8000000</v>
+        <v>15000000</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="9">
-        <v>10</v>
-      </c>
-      <c r="B28" s="9">
-        <v>6.9500000000000006E-2</v>
+        <v>20</v>
+      </c>
+      <c r="B28" s="10">
+        <v>0.02</v>
       </c>
       <c r="C28" s="8">
         <f>A28*10^6</f>
-        <v>10000000</v>
+        <v>20000000</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="9">
-        <v>15</v>
-      </c>
-      <c r="B29" s="9">
-        <v>3.3700000000000001E-2</v>
+        <v>30</v>
+      </c>
+      <c r="B29" s="10">
+        <v>9.5399999999999999E-3</v>
       </c>
       <c r="C29" s="8">
         <f>A29*10^6</f>
-        <v>15000000</v>
+        <v>30000000</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="9">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="B30" s="10">
-        <v>0.02</v>
+        <v>5.6100000000000004E-3</v>
       </c>
       <c r="C30" s="8">
         <f>A30*10^6</f>
-        <v>20000000</v>
+        <v>40000000</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="9">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="B31" s="10">
-        <v>9.5399999999999999E-3</v>
+        <v>3.7100000000000002E-3</v>
       </c>
       <c r="C31" s="8">
         <f>A31*10^6</f>
-        <v>30000000</v>
+        <v>50000000</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="9">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="B32" s="10">
-        <v>5.6100000000000004E-3</v>
+        <v>2.65E-3</v>
       </c>
       <c r="C32" s="8">
         <f>A32*10^6</f>
-        <v>40000000</v>
+        <v>60000000</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="9">
-        <v>50</v>
-      </c>
-      <c r="B33" s="10">
-        <v>3.7100000000000002E-3</v>
+        <v>80</v>
+      </c>
+      <c r="B33" s="9">
+        <v>1.5E-3</v>
       </c>
       <c r="C33" s="8">
         <f>A33*10^6</f>
-        <v>50000000</v>
+        <v>80000000</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="9">
-        <v>60</v>
-      </c>
-      <c r="B34" s="10">
-        <v>2.65E-3</v>
+        <v>100</v>
+      </c>
+      <c r="B34" s="9">
+        <v>9.6199999999999996E-4</v>
       </c>
       <c r="C34" s="8">
         <f>A34*10^6</f>
-        <v>60000000</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="9">
-        <v>80</v>
-      </c>
-      <c r="B35" s="9">
-        <v>1.5E-3</v>
-      </c>
-      <c r="C35" s="8">
-        <f>A35*10^6</f>
-        <v>80000000</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="9">
-        <v>100</v>
-      </c>
-      <c r="B36" s="9">
-        <v>9.6199999999999996E-4</v>
-      </c>
-      <c r="C36" s="8">
-        <f>A36*10^6</f>
         <v>100000000</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:B20" xr:uid="{DF36332B-B747-420B-84FA-C4CB3A896F1E}"/>
+  <autoFilter ref="A1:B18" xr:uid="{DF36332B-B747-420B-84FA-C4CB3A896F1E}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>